<commit_message>
continued to refine data sheet format
rearranged data sheet format for ease of entry/use. may need to change this later or convert to CSV when it comes time to process the data.
</commit_message>
<xml_diff>
--- a/data/tr 2019 allometric model data.xlsx
+++ b/data/tr 2019 allometric model data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissanchez/Documents/weel/tres rios/datasets/tr-allometric-modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E57BC59-D621-9847-9D73-05F751C11D46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36453FD2-5471-DF49-BA99-DE846D8F6330}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2820" windowWidth="44460" windowHeight="21420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2820" windowWidth="44460" windowHeight="21420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="typha" sheetId="2" r:id="rId1"/>
@@ -162,10 +162,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -511,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39780961-3C8A-A744-9E4D-E54E8FD78316}">
   <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
@@ -542,56 +542,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4" t="s">
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="4"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
     </row>
     <row r="2" spans="1:42" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -773,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A56EC0-1F3C-2444-8D39-08A5DAC6968F}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -792,20 +792,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6"/>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I1" s="6" t="s">

</xml_diff>